<commit_message>
updated timelog and added documentation summarization
</commit_message>
<xml_diff>
--- a/Documents/Timelogs/Timelog - Roger.xlsx
+++ b/Documents/Timelogs/Timelog - Roger.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Hours</t>
   </si>
@@ -27,12 +27,27 @@
   <si>
     <t>Roger</t>
   </si>
+  <si>
+    <t>14/9/14</t>
+  </si>
+  <si>
+    <t>Setting up the repository  computers and learning how to use git</t>
+  </si>
+  <si>
+    <t>Setting up a repository</t>
+  </si>
+  <si>
+    <t>Investigated an approach to the project with team</t>
+  </si>
+  <si>
+    <t>Summarizing Test Documents, completing python setup on computer</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -54,26 +69,12 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -171,19 +172,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
@@ -318,89 +306,109 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,6 +421,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>523876</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>885825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1" y="0"/>
+          <a:ext cx="2247900" cy="885825"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -705,7 +762,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -717,173 +774,195 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="5"/>
+      <c r="A1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="5"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="7"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="5"/>
+      <c r="A3" s="4">
+        <v>41799</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="5"/>
+      <c r="A4" s="4">
+        <v>41921</v>
+      </c>
+      <c r="B4" s="8">
+        <v>2</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="5"/>
+      <c r="A5" s="4">
+        <v>41982</v>
+      </c>
+      <c r="B5" s="8">
+        <v>2</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="5"/>
+      <c r="A6" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="8">
+        <v>5</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="5"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="5"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="5"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="7"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="5"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="7"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="5"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="7"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="5"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="7"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="5"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="7"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="5"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="7"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="5"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="7"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="5"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="7"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="5"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="7"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="5"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="7"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="5"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="7"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="5"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="7"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="5"/>
+      <c r="A21" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="7"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="5"/>
-    </row>
-    <row r="23" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-    </row>
+      <c r="C22" s="22"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>